<commit_message>
Change Design on Authorization/Authentication and Index pages, and Add KeywordStates to MedDatas
</commit_message>
<xml_diff>
--- a/src/MedAnnotateApp.Presentation/mockPMCMIDdata7.xlsx
+++ b/src/MedAnnotateApp.Presentation/mockPMCMIDdata7.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tahir\Code\MedFM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\StandfordProject\MedAnnotateApp\src\MedAnnotateApp.Presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0688C481-A463-44DD-9425-BEBC7D89542C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A98B56C-4C32-4EE3-814D-54DDB9CE7D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2265" yWindow="-21720" windowWidth="51840" windowHeight="21840" xr2:uid="{812C11EC-1E97-4F50-9AF1-2EE34443C7ED}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" xr2:uid="{812C11EC-1E97-4F50-9AF1-2EE34443C7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,12 +23,8 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -148,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="207">
   <si>
     <t>Index</t>
   </si>
@@ -842,12 +838,41 @@
   <si>
     <t>pulp stones , the upper and lower molars.</t>
   </si>
+  <si>
+    <t>https://csvc.nejm.org/ContentServer/images?id=IC20230202&amp;width=1500&amp;height=4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A previously healthy 42-year-old woman presented to the dental clinic with a 6-month history of swelling and pain on the right side of her chin (left). She reported no history of chin trauma, tooth pain, or fevers, but did recall injuring her right lateral incisor 10 years prior. Palpation of the lesion caused pain and serosanguinous fluid drainage. Intra-oral examination showed discoloration of the right lateral mandibular incisor (right). What is the most likely diagnosis?
+</t>
+  </si>
+  <si>
+    <t>Odontogenic cutaneous fistula</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>https://csvc.nejm.org/ContentServer/images?id=IC20200806&amp;width=1500&amp;height=4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 60-year-old woman presented to an oral surgery clinic with gum swelling. She had associated bleeding while brushing her teeth. She had a history of colorectal cancer treated with surgery and chemotherapy. On examination, a large, nontender, pedunculated mass was noted. What is the diagnosis?
+</t>
+  </si>
+  <si>
+    <t>gum swelling, pedunculated mass</t>
+  </si>
+  <si>
+    <t>Metastasis of colorectal cancer</t>
+  </si>
+  <si>
+    <t>right lateral incisor, Palpation of the lesion, serosanguinous fluid drainage, discoloration of the right lateral mandibular incisor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -910,6 +935,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -965,7 +996,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1009,6 +1040,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1028,7 +1060,7 @@
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <global>
     <keyFlags>
       <key name="_Self">
@@ -1453,29 +1485,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5BA7F80-C24C-40BA-AC79-3D8C6F2C8D16}">
-  <dimension ref="A1:AO12"/>
+  <dimension ref="A1:AO26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="5"/>
-    <col min="5" max="5" width="9.06640625" style="10"/>
-    <col min="11" max="11" width="28.1328125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="18.3984375" style="10" customWidth="1"/>
-    <col min="13" max="13" width="20.265625" style="10" customWidth="1"/>
-    <col min="19" max="19" width="19.86328125" style="15" customWidth="1"/>
-    <col min="20" max="20" width="18.53125" style="15" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="5"/>
+    <col min="5" max="5" width="9.109375" style="10"/>
+    <col min="11" max="11" width="28.109375" style="10" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="20.21875" style="10" customWidth="1"/>
+    <col min="19" max="19" width="19.88671875" style="15" customWidth="1"/>
+    <col min="20" max="20" width="18.5546875" style="15" customWidth="1"/>
     <col min="21" max="21" width="14.6640625" style="15" customWidth="1"/>
-    <col min="22" max="22" width="15.59765625" style="15" customWidth="1"/>
+    <col min="22" max="22" width="15.5546875" style="15" customWidth="1"/>
     <col min="23" max="23" width="14.6640625" style="15" customWidth="1"/>
-    <col min="27" max="27" width="22.3984375" style="15" customWidth="1"/>
-    <col min="32" max="32" width="16.9296875" style="15" customWidth="1"/>
+    <col min="27" max="27" width="22.44140625" style="15" customWidth="1"/>
+    <col min="32" max="32" width="16.88671875" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="157.15" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:41" ht="166.25" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
@@ -1577,7 +1609,7 @@
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
     </row>
-    <row r="2" spans="1:41" ht="285.39999999999998" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:41" ht="316.8" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1637,250 +1669,126 @@
       <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
     </row>
-    <row r="3" spans="1:41" ht="409.6" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="4">
-        <v>3433</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
+    <row r="3" spans="1:41" ht="240.9">
+      <c r="A3" s="5">
+        <v>1342</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="3" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>22</v>
+        <v>198</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U3" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="T3" s="15">
+        <v>42</v>
+      </c>
+      <c r="U3" s="15" t="s">
         <v>28</v>
       </c>
       <c r="V3" s="14" t="s">
         <v>29</v>
       </c>
       <c r="W3" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="X3" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
+        <v>200</v>
+      </c>
+      <c r="AF3" s="15" t="s">
+        <v>201</v>
+      </c>
     </row>
-    <row r="4" spans="1:41" ht="409.6" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="4">
-        <v>3436</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>34</v>
+    <row r="4" spans="1:41" ht="166.25" thickBot="1">
+      <c r="A4" s="5">
+        <v>1234</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="3" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3" t="s">
-        <v>37</v>
+        <v>202</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>38</v>
+        <v>203</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="T4" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U4" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="15">
+        <v>60</v>
+      </c>
+      <c r="U4" s="15" t="s">
         <v>28</v>
       </c>
       <c r="V4" s="14" t="s">
         <v>29</v>
       </c>
       <c r="W4" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="X4" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC4" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF4" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2"/>
-      <c r="AK4" s="2"/>
-      <c r="AL4" s="2"/>
+        <v>205</v>
+      </c>
+      <c r="AF4" s="15" t="s">
+        <v>201</v>
+      </c>
     </row>
-    <row r="5" spans="1:41" ht="409.6" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:41" ht="409.6" thickBot="1">
       <c r="A5" s="4">
-        <v>4929</v>
+        <v>3433</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="3" t="e" vm="3">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="M5" s="8"/>
+        <v>88</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="N5" s="3" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="S5" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="T5" s="14">
-        <v>50</v>
+        <v>27</v>
+      </c>
+      <c r="T5" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="U5" s="14" t="s">
         <v>28</v>
@@ -1889,87 +1797,83 @@
         <v>29</v>
       </c>
       <c r="W5" s="14" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="X5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3">
         <v>1</v>
-      </c>
-      <c r="Y5" s="3">
-        <v>0</v>
       </c>
       <c r="Z5" s="3"/>
       <c r="AA5" s="14" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="AB5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AC5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="AF5" s="14" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
       <c r="AK5" s="2"/>
       <c r="AL5" s="2"/>
     </row>
-    <row r="6" spans="1:41" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="3">
-        <v>1302459</v>
+    <row r="6" spans="1:41" ht="409.6" thickBot="1">
+      <c r="A6" s="4">
+        <v>3436</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>97</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="3" t="e" vm="4">
+        <v>35</v>
+      </c>
+      <c r="F6" s="3" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>103</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="M6" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>90</v>
+      </c>
       <c r="N6" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>115</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
       <c r="Q6" s="3" t="s">
-        <v>116</v>
+        <v>40</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>26</v>
@@ -1984,178 +1888,184 @@
         <v>28</v>
       </c>
       <c r="V6" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W6" s="14" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="X6" s="3">
         <v>0</v>
       </c>
-      <c r="Y6" s="3"/>
+      <c r="Y6" s="3">
+        <v>1</v>
+      </c>
       <c r="Z6" s="3"/>
-      <c r="AA6" s="14"/>
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
+      <c r="AA6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>1</v>
+      </c>
       <c r="AD6" s="3" t="s">
-        <v>118</v>
+        <v>32</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="AF6" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
-      <c r="AK6" s="6"/>
-      <c r="AL6" s="6"/>
-      <c r="AM6" s="6"/>
-      <c r="AN6" s="6"/>
-      <c r="AO6" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
     </row>
-    <row r="7" spans="1:41" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="3">
-        <v>1306826</v>
+    <row r="7" spans="1:41" ht="409.6" thickBot="1">
+      <c r="A7" s="4">
+        <v>4929</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F7" s="3" t="e" vm="5">
+        <v>45</v>
+      </c>
+      <c r="F7" s="3" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>109</v>
+        <v>46</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>110</v>
+        <v>47</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="M7" s="13"/>
+        <v>50</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="M7" s="8"/>
       <c r="N7" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>122</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
       <c r="Q7" s="3" t="s">
-        <v>123</v>
+        <v>52</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>124</v>
+        <v>26</v>
       </c>
       <c r="S7" s="14" t="s">
         <v>53</v>
       </c>
       <c r="T7" s="14">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="U7" s="14" t="s">
         <v>28</v>
       </c>
       <c r="V7" s="14" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="W7" s="14" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="X7" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="3">
         <v>0</v>
       </c>
-      <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
+      <c r="AA7" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>0</v>
+      </c>
       <c r="AD7" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AE7" s="3" t="s">
-        <v>126</v>
+        <v>56</v>
       </c>
       <c r="AF7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AK7" s="6"/>
-      <c r="AL7" s="6"/>
-      <c r="AM7" s="6"/>
-      <c r="AN7" s="6"/>
-      <c r="AO7" s="3"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
     </row>
-    <row r="8" spans="1:41" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:41" ht="409.6">
       <c r="A8" s="3">
-        <v>1318180</v>
+        <v>1302459</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="3" t="e" vm="6">
+        <v>100</v>
+      </c>
+      <c r="F8" s="3" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>140</v>
+        <v>191</v>
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="3" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="R8" s="3" t="s">
         <v>26</v>
@@ -2173,7 +2083,7 @@
         <v>28</v>
       </c>
       <c r="W8" s="14" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="X8" s="3">
         <v>0</v>
@@ -2184,10 +2094,10 @@
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="AE8" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="AF8" s="14" t="s">
         <v>119</v>
@@ -2198,75 +2108,75 @@
       <c r="AL8" s="6"/>
       <c r="AM8" s="6"/>
       <c r="AN8" s="6"/>
-      <c r="AO8" s="3"/>
+      <c r="AO8" s="7"/>
     </row>
-    <row r="9" spans="1:41" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:41" ht="409.6">
       <c r="A9" s="3">
-        <v>1334843</v>
+        <v>1306826</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F9" s="3" t="e" vm="7">
+        <v>108</v>
+      </c>
+      <c r="F9" s="3" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>147</v>
+        <v>193</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="M9" s="8"/>
+        <v>192</v>
+      </c>
+      <c r="M9" s="13"/>
       <c r="N9" s="3" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="S9" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="T9" s="14" t="s">
-        <v>27</v>
+        <v>53</v>
+      </c>
+      <c r="T9" s="14">
+        <v>61</v>
       </c>
       <c r="U9" s="14" t="s">
         <v>28</v>
       </c>
       <c r="V9" s="14" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="W9" s="14" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="X9" s="3">
         <v>0</v>
@@ -2277,87 +2187,89 @@
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
       <c r="AD9" s="3" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="AE9" s="3" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="AF9" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
-      <c r="AK9" s="3"/>
-      <c r="AL9" s="3"/>
-      <c r="AM9" s="3"/>
-      <c r="AN9" s="3"/>
-      <c r="AO9" s="7"/>
+      <c r="AK9" s="6"/>
+      <c r="AL9" s="6"/>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="6"/>
+      <c r="AO9" s="3"/>
     </row>
-    <row r="10" spans="1:41" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:41" ht="409.6">
       <c r="A10" s="3">
-        <v>1337514</v>
+        <v>1318180</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="F10" s="3" t="e" vm="8">
+        <v>130</v>
+      </c>
+      <c r="F10" s="3" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="I10" s="3"/>
+        <v>132</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="J10" s="3" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="3" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="S10" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="T10" s="14">
-        <v>90</v>
+        <v>27</v>
+      </c>
+      <c r="T10" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="U10" s="14" t="s">
         <v>28</v>
       </c>
       <c r="V10" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W10" s="14" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="X10" s="3">
         <v>0</v>
@@ -2368,13 +2280,13 @@
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
       <c r="AD10" s="3" t="s">
-        <v>165</v>
+        <v>58</v>
       </c>
       <c r="AE10" s="3" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="AF10" s="14" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
@@ -2382,60 +2294,60 @@
       <c r="AL10" s="6"/>
       <c r="AM10" s="6"/>
       <c r="AN10" s="6"/>
-      <c r="AO10" s="7"/>
+      <c r="AO10" s="3"/>
     </row>
-    <row r="11" spans="1:41" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:41" ht="409.6">
       <c r="A11" s="3">
-        <v>1365911</v>
+        <v>1334843</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>168</v>
+        <v>95</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="F11" s="3" t="e" vm="9">
+        <v>143</v>
+      </c>
+      <c r="F11" s="3" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>170</v>
+        <v>144</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="M11" s="13"/>
+        <v>194</v>
+      </c>
+      <c r="M11" s="8"/>
       <c r="N11" s="3" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="R11" s="3" t="e">
-        <v>#NAME?</v>
+        <v>151</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="S11" s="14" t="s">
         <v>27</v>
@@ -2447,10 +2359,10 @@
         <v>28</v>
       </c>
       <c r="V11" s="14" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="W11" s="14" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="X11" s="3">
         <v>0</v>
@@ -2461,76 +2373,78 @@
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AE11" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AF11" s="14" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="AG11" s="3"/>
-      <c r="AH11" s="6"/>
-      <c r="AK11" s="6"/>
-      <c r="AL11" s="6"/>
-      <c r="AM11" s="6"/>
-      <c r="AN11" s="6"/>
+      <c r="AH11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="3"/>
       <c r="AO11" s="7"/>
     </row>
-    <row r="12" spans="1:41" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:41" ht="409.6">
       <c r="A12" s="3">
-        <v>1375972</v>
+        <v>1337514</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>180</v>
+        <v>153</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>94</v>
+        <v>154</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="F12" s="3" t="e" vm="10">
+        <v>155</v>
+      </c>
+      <c r="F12" s="3" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M12" s="13"/>
       <c r="N12" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="P12" s="3"/>
+        <v>160</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="Q12" s="3" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="R12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="S12" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="T12" s="14" t="s">
-        <v>27</v>
+        <v>53</v>
+      </c>
+      <c r="T12" s="14">
+        <v>90</v>
       </c>
       <c r="U12" s="14" t="s">
         <v>28</v>
@@ -2539,7 +2453,7 @@
         <v>29</v>
       </c>
       <c r="W12" s="14" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="X12" s="3">
         <v>0</v>
@@ -2550,13 +2464,13 @@
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="AE12" s="3" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="AF12" s="14" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
@@ -2566,20 +2480,242 @@
       <c r="AN12" s="6"/>
       <c r="AO12" s="7"/>
     </row>
+    <row r="13" spans="1:41" ht="409.6">
+      <c r="A13" s="3">
+        <v>1365911</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="3" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="M13" s="13"/>
+      <c r="N13" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="R13" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="S13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="T13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="U13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="V13" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="W13" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="X13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="14"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="6"/>
+      <c r="AK13" s="6"/>
+      <c r="AL13" s="6"/>
+      <c r="AM13" s="6"/>
+      <c r="AN13" s="6"/>
+      <c r="AO13" s="7"/>
+    </row>
+    <row r="14" spans="1:41" ht="409.6">
+      <c r="A14" s="3">
+        <v>1375972</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="F14" s="3" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="M14" s="13"/>
+      <c r="N14" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="T14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="U14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="V14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="W14" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="X14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="AE14" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="AF14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AK14" s="6"/>
+      <c r="AL14" s="6"/>
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="7"/>
+    </row>
+    <row r="15" spans="1:41" ht="335.3" customHeight="1">
+      <c r="E15" s="17"/>
+    </row>
+    <row r="16" spans="1:41">
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" spans="5:5">
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="5:5">
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="5:5">
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" spans="5:5">
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="5:5">
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="5:5">
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="5:5">
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="5:5">
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="5:5">
+      <c r="E26" s="17"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1" display="https://docs.google.com/document/d/1H5zIw7IsmjNivWyMFnPk0hxoh24SX4qgGLdkQLevrNw/edit?usp=sharing" xr:uid="{74E30486-1792-4849-9763-75A2A080635E}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{A0C10CAB-3B06-4E8A-825A-E2966CAA3460}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{75B147A1-0BFD-4F13-B107-1C4E826977EC}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{DB9E4A22-11B7-4EE0-9379-125FBF48302B}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{A195EF5D-E918-41D0-9AF3-8A03E5313051}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{F2D5DC82-4276-4129-9D82-773CF1647B63}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{306938E1-0E46-42B2-8A85-9E2ECD7EF34E}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{139A5349-0CCF-4D05-A6D4-921EC97AEFCB}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{A62CC7BD-73FB-4FBB-AFC1-396AEF4DC7A2}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{A2152F16-0492-4810-84C0-43D5FA257214}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{F8DC0C41-5C09-4610-956A-09C0A3CBED98}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{A0C10CAB-3B06-4E8A-825A-E2966CAA3460}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{75B147A1-0BFD-4F13-B107-1C4E826977EC}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{DB9E4A22-11B7-4EE0-9379-125FBF48302B}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{A195EF5D-E918-41D0-9AF3-8A03E5313051}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{F2D5DC82-4276-4129-9D82-773CF1647B63}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{306938E1-0E46-42B2-8A85-9E2ECD7EF34E}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{139A5349-0CCF-4D05-A6D4-921EC97AEFCB}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{A62CC7BD-73FB-4FBB-AFC1-396AEF4DC7A2}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{A2152F16-0492-4810-84C0-43D5FA257214}"/>
+    <hyperlink ref="E14" r:id="rId11" xr:uid="{F8DC0C41-5C09-4610-956A-09C0A3CBED98}"/>
+    <hyperlink ref="E3" r:id="rId12" xr:uid="{AC7ACCDC-B321-489F-8505-80BCC4B1BAB1}"/>
+    <hyperlink ref="E4" r:id="rId13" xr:uid="{168C8878-49FC-459D-86E9-CB1ADF104F33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>